<commit_message>
Few fixes after reviews.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_pooling_v3_12_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_pooling_v3_12_0.xlsx
@@ -33,6 +33,9 @@
     <t xml:space="preserve">3.12.0</t>
   </si>
   <si>
+    <t xml:space="preserve">Pool Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source Sample Name</t>
   </si>
   <si>
@@ -40,9 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">Source Container Coord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool Name</t>
   </si>
   <si>
     <t xml:space="preserve">Source Depleted</t>
@@ -1809,6 +1809,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1818,10 +1822,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1841,15 +1841,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2030,23 +2030,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W710"/>
+  <dimension ref="A1:V710"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="9" style="0" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="8" style="0" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,17 +2069,17 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="W5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="V5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="W6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="V6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
@@ -2089,10 +2088,10 @@
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="9" t="s">
@@ -2116,8 +2115,8 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="15"/>
       <c r="F9" s="18"/>
@@ -2125,8 +2124,8 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="15"/>
       <c r="F10" s="18"/>
@@ -2134,8 +2133,8 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
       <c r="F11" s="18"/>
@@ -2143,8 +2142,8 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="15"/>
       <c r="F12" s="18"/>
@@ -2152,8 +2151,8 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
       <c r="F13" s="18"/>
@@ -2161,8 +2160,8 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
       <c r="F14" s="18"/>
@@ -2170,8 +2169,8 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="15"/>
       <c r="F15" s="18"/>
@@ -2179,8 +2178,8 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
       <c r="F16" s="18"/>
@@ -2188,8 +2187,8 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="15"/>
       <c r="F17" s="18"/>
@@ -2197,8 +2196,8 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
       <c r="F18" s="18"/>
@@ -2206,8 +2205,8 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
       <c r="F19" s="18"/>
@@ -2215,8 +2214,8 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
       <c r="F20" s="18"/>
@@ -2224,8 +2223,8 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="15"/>
       <c r="F21" s="18"/>
@@ -2233,8 +2232,8 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
       <c r="F22" s="18"/>
@@ -2242,8 +2241,8 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
       <c r="F23" s="18"/>
@@ -2251,8 +2250,8 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
       <c r="F24" s="18"/>
@@ -2260,8 +2259,8 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="18"/>
@@ -2269,8 +2268,8 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="15"/>
       <c r="F26" s="18"/>
@@ -2278,8 +2277,8 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="15"/>
       <c r="F27" s="18"/>
@@ -2287,8 +2286,8 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="15"/>
       <c r="F28" s="18"/>
@@ -2296,8 +2295,8 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="15"/>
       <c r="F29" s="18"/>
@@ -2305,8 +2304,8 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="15"/>
       <c r="F30" s="18"/>
@@ -2314,8 +2313,8 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="15"/>
       <c r="F31" s="18"/>
@@ -2323,8 +2322,8 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="15"/>
       <c r="F32" s="18"/>
@@ -2332,8 +2331,8 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="15"/>
       <c r="F33" s="18"/>
@@ -2341,8 +2340,8 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="15"/>
       <c r="F34" s="18"/>
@@ -2350,8 +2349,8 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="15"/>
       <c r="F35" s="18"/>
@@ -2359,8 +2358,8 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="11"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="15"/>
       <c r="F36" s="18"/>
@@ -2368,8 +2367,8 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="11"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="15"/>
       <c r="F37" s="18"/>
@@ -2377,8 +2376,8 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="15"/>
       <c r="F38" s="18"/>
@@ -2386,8 +2385,8 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="15"/>
       <c r="F39" s="18"/>
@@ -2395,8 +2394,8 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="15"/>
       <c r="F40" s="18"/>
@@ -2404,8 +2403,8 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="15"/>
       <c r="F41" s="18"/>
@@ -2413,8 +2412,8 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="15"/>
       <c r="F42" s="18"/>
@@ -2422,8 +2421,8 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="15"/>
       <c r="F43" s="18"/>
@@ -2431,8 +2430,8 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="15"/>
       <c r="F44" s="18"/>
@@ -2440,8 +2439,8 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="15"/>
       <c r="F45" s="18"/>
@@ -2449,8 +2448,8 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="14"/>
       <c r="D46" s="14"/>
       <c r="E46" s="15"/>
       <c r="F46" s="18"/>
@@ -2458,8 +2457,8 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="15"/>
       <c r="F47" s="18"/>
@@ -2467,8 +2466,8 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="15"/>
       <c r="F48" s="18"/>
@@ -2476,8 +2475,8 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="E49" s="15"/>
       <c r="F49" s="18"/>
@@ -2485,8 +2484,8 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="15"/>
       <c r="F50" s="18"/>
@@ -2494,8 +2493,8 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="15"/>
       <c r="F51" s="18"/>
@@ -2503,8 +2502,8 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="15"/>
       <c r="F52" s="18"/>
@@ -2512,8 +2511,8 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="15"/>
       <c r="F53" s="18"/>
@@ -2521,8 +2520,8 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="15"/>
       <c r="F54" s="18"/>
@@ -2530,8 +2529,8 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="E55" s="15"/>
       <c r="F55" s="18"/>
@@ -2539,8 +2538,8 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="11"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="15"/>
       <c r="F56" s="18"/>
@@ -2548,8 +2547,8 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="11"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="15"/>
       <c r="F57" s="18"/>
@@ -2557,8 +2556,8 @@
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="11"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="15"/>
       <c r="F58" s="18"/>
@@ -2566,8 +2565,8 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="11"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="15"/>
       <c r="F59" s="18"/>
@@ -2575,8 +2574,8 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="11"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="15"/>
       <c r="F60" s="18"/>
@@ -2584,8 +2583,8 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="11"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="15"/>
       <c r="F61" s="18"/>
@@ -2593,8 +2592,8 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="11"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="15"/>
       <c r="F62" s="18"/>
@@ -2602,8 +2601,8 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="11"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="15"/>
       <c r="F63" s="18"/>
@@ -2611,8 +2610,8 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="11"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="15"/>
       <c r="F64" s="18"/>
@@ -2620,8 +2619,8 @@
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="11"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="15"/>
       <c r="F65" s="18"/>
@@ -2629,8 +2628,8 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="11"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="15"/>
       <c r="F66" s="18"/>
@@ -2638,8 +2637,8 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="11"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="15"/>
       <c r="F67" s="18"/>
@@ -2647,8 +2646,8 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="11"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="15"/>
       <c r="F68" s="18"/>
@@ -2656,8 +2655,8 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="11"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="15"/>
       <c r="F69" s="18"/>
@@ -2665,8 +2664,8 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="11"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="15"/>
       <c r="F70" s="18"/>
@@ -2674,8 +2673,8 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="11"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="15"/>
       <c r="F71" s="18"/>
@@ -2683,8 +2682,8 @@
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="11"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="15"/>
       <c r="F72" s="18"/>
@@ -2692,8 +2691,8 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="11"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="15"/>
       <c r="F73" s="18"/>
@@ -2701,8 +2700,8 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="11"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="15"/>
       <c r="F74" s="18"/>
@@ -2710,8 +2709,8 @@
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="11"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="15"/>
       <c r="F75" s="18"/>
@@ -2719,8 +2718,8 @@
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="11"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="15"/>
       <c r="F76" s="18"/>
@@ -2728,8 +2727,8 @@
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="11"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="14"/>
       <c r="E77" s="15"/>
       <c r="F77" s="18"/>
@@ -2737,8 +2736,8 @@
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="11"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="14"/>
       <c r="D78" s="14"/>
       <c r="E78" s="15"/>
       <c r="F78" s="18"/>
@@ -2746,8 +2745,8 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="11"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="14"/>
       <c r="D79" s="14"/>
       <c r="E79" s="15"/>
       <c r="F79" s="18"/>
@@ -2755,8 +2754,8 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="11"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="14"/>
       <c r="E80" s="15"/>
       <c r="F80" s="18"/>
@@ -2764,8 +2763,8 @@
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="11"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="14"/>
       <c r="E81" s="15"/>
       <c r="F81" s="18"/>
@@ -2773,8 +2772,8 @@
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="11"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="14"/>
       <c r="E82" s="15"/>
       <c r="F82" s="18"/>
@@ -2782,8 +2781,8 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="11"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="14"/>
       <c r="E83" s="15"/>
       <c r="F83" s="18"/>
@@ -2791,8 +2790,8 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="11"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="14"/>
       <c r="D84" s="14"/>
       <c r="E84" s="15"/>
       <c r="F84" s="18"/>
@@ -2800,8 +2799,8 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="11"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="E85" s="15"/>
       <c r="F85" s="18"/>
@@ -2809,8 +2808,8 @@
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="11"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="14"/>
       <c r="D86" s="14"/>
       <c r="E86" s="15"/>
       <c r="F86" s="18"/>
@@ -2818,8 +2817,8 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="11"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="14"/>
       <c r="D87" s="14"/>
       <c r="E87" s="15"/>
       <c r="F87" s="18"/>
@@ -2827,8 +2826,8 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="11"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="14"/>
       <c r="D88" s="14"/>
       <c r="E88" s="15"/>
       <c r="F88" s="18"/>
@@ -2836,8 +2835,8 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="11"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="14"/>
       <c r="D89" s="14"/>
       <c r="E89" s="15"/>
       <c r="F89" s="18"/>
@@ -2845,8 +2844,8 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="11"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="14"/>
       <c r="D90" s="14"/>
       <c r="E90" s="15"/>
       <c r="F90" s="18"/>
@@ -2854,8 +2853,8 @@
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="11"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="14"/>
       <c r="D91" s="14"/>
       <c r="E91" s="15"/>
       <c r="F91" s="18"/>
@@ -2863,8 +2862,8 @@
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="11"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="15"/>
       <c r="F92" s="18"/>
@@ -2872,8 +2871,8 @@
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="15"/>
       <c r="F93" s="18"/>
@@ -2881,8 +2880,8 @@
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="11"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="15"/>
       <c r="F94" s="18"/>
@@ -2890,8 +2889,8 @@
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="11"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="14"/>
       <c r="D95" s="14"/>
       <c r="E95" s="15"/>
       <c r="F95" s="18"/>
@@ -2899,8 +2898,8 @@
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="11"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="14"/>
       <c r="D96" s="14"/>
       <c r="E96" s="15"/>
       <c r="F96" s="18"/>
@@ -2908,8 +2907,8 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="11"/>
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="14"/>
       <c r="E97" s="15"/>
       <c r="F97" s="18"/>
@@ -2917,8 +2916,8 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="11"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="14"/>
       <c r="E98" s="15"/>
       <c r="F98" s="18"/>
@@ -2926,8 +2925,8 @@
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="11"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="14"/>
       <c r="D99" s="14"/>
       <c r="E99" s="15"/>
       <c r="F99" s="18"/>
@@ -2935,8 +2934,8 @@
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="11"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="14"/>
       <c r="D100" s="14"/>
       <c r="E100" s="15"/>
       <c r="F100" s="18"/>
@@ -2944,8 +2943,8 @@
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="11"/>
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="14"/>
       <c r="E101" s="15"/>
       <c r="F101" s="18"/>
@@ -2953,8 +2952,8 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="11"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="B102" s="12"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="14"/>
       <c r="E102" s="15"/>
       <c r="F102" s="18"/>
@@ -2963,7 +2962,7 @@
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="19"/>
       <c r="B103" s="20"/>
-      <c r="C103" s="20"/>
+      <c r="C103" s="21"/>
       <c r="D103" s="21"/>
       <c r="E103" s="22"/>
       <c r="F103" s="23"/>
@@ -3578,11 +3577,11 @@
     <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C8:C103" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D8:D103" type="list">
       <formula1>Index!$A$2:$A$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D8:D103" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A8:A103" type="list">
       <formula1>Pools!$A$4:$A$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3612,7 +3611,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
@@ -3621,7 +3620,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.57"/>
   </cols>
   <sheetData>
@@ -3632,7 +3631,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>10</v>
@@ -3673,8 +3672,8 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29"/>
       <c r="B5" s="37"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="32"/>
       <c r="F5" s="38"/>
       <c r="G5" s="34"/>
@@ -3684,8 +3683,8 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29"/>
       <c r="B6" s="37"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="32"/>
       <c r="F6" s="38"/>
       <c r="G6" s="34"/>
@@ -3695,8 +3694,8 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29"/>
       <c r="B7" s="37"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="32"/>
       <c r="F7" s="38"/>
       <c r="G7" s="34"/>
@@ -3706,8 +3705,8 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29"/>
       <c r="B8" s="37"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="32"/>
       <c r="F8" s="38"/>
       <c r="G8" s="34"/>
@@ -3717,8 +3716,8 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29"/>
       <c r="B9" s="37"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="32"/>
       <c r="F9" s="38"/>
       <c r="G9" s="34"/>
@@ -3728,8 +3727,8 @@
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29"/>
       <c r="B10" s="37"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="32"/>
       <c r="F10" s="38"/>
       <c r="G10" s="34"/>
@@ -3739,8 +3738,8 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="37"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="32"/>
       <c r="F11" s="38"/>
       <c r="G11" s="34"/>
@@ -3750,8 +3749,8 @@
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="37"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="32"/>
       <c r="F12" s="38"/>
       <c r="G12" s="34"/>
@@ -3761,8 +3760,8 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="37"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="32"/>
       <c r="F13" s="38"/>
       <c r="G13" s="34"/>
@@ -3772,8 +3771,8 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="37"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="32"/>
       <c r="F14" s="38"/>
       <c r="G14" s="34"/>
@@ -3783,8 +3782,8 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="37"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="32"/>
       <c r="F15" s="38"/>
       <c r="G15" s="34"/>
@@ -3794,8 +3793,8 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="32"/>
       <c r="F16" s="38"/>
       <c r="G16" s="34"/>
@@ -3805,8 +3804,8 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="37"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="32"/>
       <c r="F17" s="38"/>
       <c r="G17" s="34"/>
@@ -3816,8 +3815,8 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="37"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="32"/>
       <c r="F18" s="38"/>
       <c r="G18" s="34"/>
@@ -3827,8 +3826,8 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="37"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="32"/>
       <c r="F19" s="38"/>
       <c r="G19" s="34"/>
@@ -3838,8 +3837,8 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29"/>
       <c r="B20" s="37"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="32"/>
       <c r="F20" s="38"/>
       <c r="G20" s="34"/>
@@ -3849,8 +3848,8 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="29"/>
       <c r="B21" s="37"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="32"/>
       <c r="F21" s="38"/>
       <c r="G21" s="34"/>
@@ -3860,8 +3859,8 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="29"/>
       <c r="B22" s="37"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="32"/>
       <c r="F22" s="38"/>
       <c r="G22" s="34"/>
@@ -3871,8 +3870,8 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29"/>
       <c r="B23" s="37"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="32"/>
       <c r="F23" s="38"/>
       <c r="G23" s="34"/>
@@ -3882,8 +3881,8 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="29"/>
       <c r="B24" s="37"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="32"/>
       <c r="F24" s="38"/>
       <c r="G24" s="34"/>
@@ -3893,8 +3892,8 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29"/>
       <c r="B25" s="37"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="32"/>
       <c r="F25" s="38"/>
       <c r="G25" s="34"/>
@@ -3904,8 +3903,8 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="29"/>
       <c r="B26" s="37"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="32"/>
       <c r="F26" s="38"/>
       <c r="G26" s="34"/>
@@ -3915,8 +3914,8 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="29"/>
       <c r="B27" s="37"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="32"/>
       <c r="F27" s="38"/>
       <c r="G27" s="34"/>
@@ -3926,8 +3925,8 @@
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="29"/>
       <c r="B28" s="37"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="32"/>
       <c r="F28" s="38"/>
       <c r="G28" s="34"/>
@@ -3937,8 +3936,8 @@
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="29"/>
       <c r="B29" s="37"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="32"/>
       <c r="F29" s="38"/>
       <c r="G29" s="34"/>
@@ -3948,8 +3947,8 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="29"/>
       <c r="B30" s="37"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="32"/>
       <c r="F30" s="38"/>
       <c r="G30" s="34"/>
@@ -3959,8 +3958,8 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="29"/>
       <c r="B31" s="37"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="32"/>
       <c r="F31" s="38"/>
       <c r="G31" s="34"/>
@@ -3970,8 +3969,8 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29"/>
       <c r="B32" s="37"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="32"/>
       <c r="F32" s="38"/>
       <c r="G32" s="34"/>
@@ -3981,8 +3980,8 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29"/>
       <c r="B33" s="37"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="32"/>
       <c r="F33" s="38"/>
       <c r="G33" s="34"/>
@@ -3992,8 +3991,8 @@
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="29"/>
       <c r="B34" s="37"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="32"/>
       <c r="F34" s="38"/>
       <c r="G34" s="34"/>
@@ -4003,8 +4002,8 @@
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="29"/>
       <c r="B35" s="37"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="32"/>
       <c r="F35" s="38"/>
       <c r="G35" s="34"/>
@@ -4014,8 +4013,8 @@
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="29"/>
       <c r="B36" s="37"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="32"/>
       <c r="F36" s="38"/>
       <c r="G36" s="34"/>
@@ -4025,8 +4024,8 @@
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29"/>
       <c r="B37" s="37"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="32"/>
       <c r="F37" s="38"/>
       <c r="G37" s="34"/>
@@ -4036,8 +4035,8 @@
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="29"/>
       <c r="B38" s="37"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="32"/>
       <c r="F38" s="38"/>
       <c r="G38" s="34"/>
@@ -4047,8 +4046,8 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="29"/>
       <c r="B39" s="37"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="32"/>
       <c r="F39" s="38"/>
       <c r="G39" s="34"/>
@@ -4058,8 +4057,8 @@
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="29"/>
       <c r="B40" s="37"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="32"/>
       <c r="F40" s="38"/>
       <c r="G40" s="34"/>
@@ -4069,8 +4068,8 @@
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="29"/>
       <c r="B41" s="37"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="32"/>
       <c r="F41" s="38"/>
       <c r="G41" s="34"/>
@@ -4080,8 +4079,8 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="29"/>
       <c r="B42" s="37"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="32"/>
       <c r="F42" s="38"/>
       <c r="G42" s="34"/>
@@ -4091,8 +4090,8 @@
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="29"/>
       <c r="B43" s="37"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="32"/>
       <c r="F43" s="38"/>
       <c r="G43" s="34"/>
@@ -4102,8 +4101,8 @@
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="29"/>
       <c r="B44" s="37"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="32"/>
       <c r="F44" s="38"/>
       <c r="G44" s="34"/>
@@ -4113,8 +4112,8 @@
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="29"/>
       <c r="B45" s="37"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
       <c r="E45" s="32"/>
       <c r="F45" s="38"/>
       <c r="G45" s="34"/>
@@ -4124,8 +4123,8 @@
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="29"/>
       <c r="B46" s="37"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
       <c r="E46" s="32"/>
       <c r="F46" s="38"/>
       <c r="G46" s="34"/>
@@ -4135,8 +4134,8 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="29"/>
       <c r="B47" s="37"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
       <c r="E47" s="32"/>
       <c r="F47" s="38"/>
       <c r="G47" s="34"/>
@@ -4146,8 +4145,8 @@
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="29"/>
       <c r="B48" s="37"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
       <c r="E48" s="32"/>
       <c r="F48" s="38"/>
       <c r="G48" s="34"/>
@@ -4157,8 +4156,8 @@
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="29"/>
       <c r="B49" s="37"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="32"/>
       <c r="F49" s="38"/>
       <c r="G49" s="34"/>
@@ -4168,8 +4167,8 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="29"/>
       <c r="B50" s="37"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="32"/>
       <c r="F50" s="38"/>
       <c r="G50" s="34"/>
@@ -4179,8 +4178,8 @@
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="29"/>
       <c r="B51" s="37"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="32"/>
       <c r="F51" s="38"/>
       <c r="G51" s="34"/>
@@ -4190,8 +4189,8 @@
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="29"/>
       <c r="B52" s="37"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
       <c r="E52" s="32"/>
       <c r="F52" s="38"/>
       <c r="G52" s="34"/>
@@ -4201,8 +4200,8 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="29"/>
       <c r="B53" s="37"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="32"/>
       <c r="F53" s="38"/>
       <c r="G53" s="34"/>
@@ -4212,8 +4211,8 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="29"/>
       <c r="B54" s="37"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
       <c r="E54" s="32"/>
       <c r="F54" s="38"/>
       <c r="G54" s="34"/>
@@ -4223,8 +4222,8 @@
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="29"/>
       <c r="B55" s="37"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
       <c r="E55" s="32"/>
       <c r="F55" s="38"/>
       <c r="G55" s="34"/>
@@ -4234,8 +4233,8 @@
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="29"/>
       <c r="B56" s="37"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
       <c r="E56" s="32"/>
       <c r="F56" s="38"/>
       <c r="G56" s="34"/>
@@ -4245,8 +4244,8 @@
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="29"/>
       <c r="B57" s="37"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
       <c r="E57" s="32"/>
       <c r="F57" s="38"/>
       <c r="G57" s="34"/>
@@ -4256,8 +4255,8 @@
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="29"/>
       <c r="B58" s="37"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
       <c r="E58" s="32"/>
       <c r="F58" s="38"/>
       <c r="G58" s="34"/>
@@ -4267,8 +4266,8 @@
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="29"/>
       <c r="B59" s="37"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
       <c r="E59" s="32"/>
       <c r="F59" s="38"/>
       <c r="G59" s="34"/>
@@ -4278,8 +4277,8 @@
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="29"/>
       <c r="B60" s="37"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
       <c r="E60" s="32"/>
       <c r="F60" s="38"/>
       <c r="G60" s="34"/>
@@ -4289,8 +4288,8 @@
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="29"/>
       <c r="B61" s="37"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
       <c r="E61" s="32"/>
       <c r="F61" s="38"/>
       <c r="G61" s="34"/>
@@ -4300,8 +4299,8 @@
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="29"/>
       <c r="B62" s="37"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
       <c r="E62" s="32"/>
       <c r="F62" s="38"/>
       <c r="G62" s="34"/>
@@ -4311,8 +4310,8 @@
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="29"/>
       <c r="B63" s="37"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
       <c r="E63" s="32"/>
       <c r="F63" s="38"/>
       <c r="G63" s="34"/>
@@ -4322,8 +4321,8 @@
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="29"/>
       <c r="B64" s="37"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
       <c r="E64" s="32"/>
       <c r="F64" s="38"/>
       <c r="G64" s="34"/>
@@ -4333,8 +4332,8 @@
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="29"/>
       <c r="B65" s="37"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
       <c r="E65" s="32"/>
       <c r="F65" s="38"/>
       <c r="G65" s="34"/>
@@ -4344,8 +4343,8 @@
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="29"/>
       <c r="B66" s="37"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
       <c r="E66" s="32"/>
       <c r="F66" s="38"/>
       <c r="G66" s="34"/>
@@ -4355,8 +4354,8 @@
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="29"/>
       <c r="B67" s="37"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
       <c r="E67" s="32"/>
       <c r="F67" s="38"/>
       <c r="G67" s="34"/>
@@ -4366,8 +4365,8 @@
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="29"/>
       <c r="B68" s="37"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
       <c r="E68" s="32"/>
       <c r="F68" s="38"/>
       <c r="G68" s="34"/>
@@ -4377,8 +4376,8 @@
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="29"/>
       <c r="B69" s="37"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
       <c r="E69" s="32"/>
       <c r="F69" s="38"/>
       <c r="G69" s="34"/>
@@ -4388,8 +4387,8 @@
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="29"/>
       <c r="B70" s="37"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
       <c r="E70" s="32"/>
       <c r="F70" s="38"/>
       <c r="G70" s="34"/>
@@ -4399,8 +4398,8 @@
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="29"/>
       <c r="B71" s="37"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
       <c r="E71" s="32"/>
       <c r="F71" s="38"/>
       <c r="G71" s="34"/>
@@ -4410,8 +4409,8 @@
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="29"/>
       <c r="B72" s="37"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
       <c r="E72" s="32"/>
       <c r="F72" s="38"/>
       <c r="G72" s="34"/>
@@ -4421,8 +4420,8 @@
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="29"/>
       <c r="B73" s="37"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
       <c r="E73" s="32"/>
       <c r="F73" s="38"/>
       <c r="G73" s="34"/>
@@ -4432,8 +4431,8 @@
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="29"/>
       <c r="B74" s="37"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
       <c r="E74" s="32"/>
       <c r="F74" s="38"/>
       <c r="G74" s="34"/>
@@ -4443,8 +4442,8 @@
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="29"/>
       <c r="B75" s="37"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
       <c r="E75" s="32"/>
       <c r="F75" s="38"/>
       <c r="G75" s="34"/>
@@ -4454,8 +4453,8 @@
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="29"/>
       <c r="B76" s="37"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
       <c r="E76" s="32"/>
       <c r="F76" s="38"/>
       <c r="G76" s="34"/>
@@ -4465,8 +4464,8 @@
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="29"/>
       <c r="B77" s="37"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
       <c r="E77" s="32"/>
       <c r="F77" s="38"/>
       <c r="G77" s="34"/>
@@ -4476,8 +4475,8 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="29"/>
       <c r="B78" s="37"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
       <c r="E78" s="32"/>
       <c r="F78" s="38"/>
       <c r="G78" s="34"/>
@@ -4487,8 +4486,8 @@
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="29"/>
       <c r="B79" s="37"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
       <c r="E79" s="32"/>
       <c r="F79" s="38"/>
       <c r="G79" s="34"/>
@@ -4498,8 +4497,8 @@
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="29"/>
       <c r="B80" s="37"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
       <c r="E80" s="32"/>
       <c r="F80" s="38"/>
       <c r="G80" s="34"/>
@@ -4509,8 +4508,8 @@
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="29"/>
       <c r="B81" s="37"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
       <c r="E81" s="32"/>
       <c r="F81" s="38"/>
       <c r="G81" s="34"/>
@@ -4520,8 +4519,8 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="29"/>
       <c r="B82" s="37"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
       <c r="E82" s="32"/>
       <c r="F82" s="38"/>
       <c r="G82" s="34"/>
@@ -4531,8 +4530,8 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="29"/>
       <c r="B83" s="37"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
       <c r="E83" s="32"/>
       <c r="F83" s="38"/>
       <c r="G83" s="34"/>
@@ -4542,8 +4541,8 @@
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="29"/>
       <c r="B84" s="37"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
       <c r="E84" s="32"/>
       <c r="F84" s="38"/>
       <c r="G84" s="34"/>
@@ -4553,8 +4552,8 @@
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="29"/>
       <c r="B85" s="37"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
       <c r="E85" s="32"/>
       <c r="F85" s="38"/>
       <c r="G85" s="34"/>
@@ -4564,8 +4563,8 @@
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="29"/>
       <c r="B86" s="37"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
       <c r="E86" s="32"/>
       <c r="F86" s="38"/>
       <c r="G86" s="34"/>
@@ -4575,8 +4574,8 @@
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="29"/>
       <c r="B87" s="37"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
       <c r="E87" s="32"/>
       <c r="F87" s="38"/>
       <c r="G87" s="34"/>
@@ -4586,8 +4585,8 @@
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="29"/>
       <c r="B88" s="37"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
       <c r="E88" s="32"/>
       <c r="F88" s="38"/>
       <c r="G88" s="34"/>
@@ -4597,8 +4596,8 @@
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="29"/>
       <c r="B89" s="37"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
       <c r="E89" s="32"/>
       <c r="F89" s="38"/>
       <c r="G89" s="34"/>
@@ -4608,8 +4607,8 @@
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="29"/>
       <c r="B90" s="37"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
       <c r="E90" s="32"/>
       <c r="F90" s="38"/>
       <c r="G90" s="34"/>
@@ -4619,8 +4618,8 @@
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="29"/>
       <c r="B91" s="37"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
       <c r="E91" s="32"/>
       <c r="F91" s="38"/>
       <c r="G91" s="34"/>
@@ -4630,8 +4629,8 @@
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="29"/>
       <c r="B92" s="37"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
       <c r="E92" s="32"/>
       <c r="F92" s="38"/>
       <c r="G92" s="34"/>
@@ -4641,8 +4640,8 @@
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="29"/>
       <c r="B93" s="37"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
       <c r="E93" s="32"/>
       <c r="F93" s="38"/>
       <c r="G93" s="34"/>
@@ -4652,8 +4651,8 @@
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="29"/>
       <c r="B94" s="37"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
       <c r="E94" s="32"/>
       <c r="F94" s="38"/>
       <c r="G94" s="34"/>
@@ -4663,8 +4662,8 @@
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="29"/>
       <c r="B95" s="37"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
       <c r="E95" s="32"/>
       <c r="F95" s="38"/>
       <c r="G95" s="34"/>
@@ -4674,8 +4673,8 @@
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="29"/>
       <c r="B96" s="37"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="14"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
       <c r="E96" s="32"/>
       <c r="F96" s="38"/>
       <c r="G96" s="34"/>
@@ -4685,8 +4684,8 @@
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="29"/>
       <c r="B97" s="37"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
       <c r="E97" s="32"/>
       <c r="F97" s="38"/>
       <c r="G97" s="34"/>
@@ -4696,8 +4695,8 @@
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="29"/>
       <c r="B98" s="37"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="14"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
       <c r="E98" s="32"/>
       <c r="F98" s="38"/>
       <c r="G98" s="34"/>
@@ -4707,8 +4706,8 @@
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="39"/>
       <c r="B99" s="40"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
       <c r="E99" s="41"/>
       <c r="F99" s="42"/>
       <c r="G99" s="43"/>
@@ -4747,11 +4746,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="6" style="0" width="9.33"/>
   </cols>

</xml_diff>